<commit_message>
Major changes in WA messages, WA bot, spravka
</commit_message>
<xml_diff>
--- a/staticfiles/user_manager/students.xlsx
+++ b/staticfiles/user_manager/students.xlsx
@@ -475,7 +475,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,28 +541,118 @@
       </c>
       <c r="B2" s="4" t="inlineStr">
         <is>
-          <t>dAS asd SAD</t>
+          <t>erwyg dfgs dfgs</t>
         </is>
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>242341324234</t>
-        </is>
-      </c>
-      <c r="D2" s="4" t="n"/>
-      <c r="E2" s="4" t="n"/>
-      <c r="F2" s="4" t="n"/>
-      <c r="G2" s="4" t="n"/>
+          <t>856477567657</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t>dfsa ddafs asdf</t>
+        </is>
+      </c>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>+7 (132) 412-34-31</t>
+        </is>
+      </c>
+      <c r="F2" s="4" t="inlineStr">
+        <is>
+          <t>sadf</t>
+        </is>
+      </c>
+      <c r="G2" s="4" t="n">
+        <v>3124</v>
+      </c>
       <c r="H2" s="4" t="inlineStr">
         <is>
-          <t>9 A</t>
+          <t>3 Б</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="F5" s="5" t="inlineStr">
-        <is>
-          <t>Все классы - 1 учеников</t>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dolmagambetov Karen </t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>010608550491</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="inlineStr">
+        <is>
+          <t>Долмагамбетов Талгат Аманжолович</t>
+        </is>
+      </c>
+      <c r="E3" s="4" t="inlineStr">
+        <is>
+          <t>+7 (771) 168-86-87</t>
+        </is>
+      </c>
+      <c r="F3" s="4" t="inlineStr">
+        <is>
+          <t>214234</t>
+        </is>
+      </c>
+      <c r="G3" s="4" t="n">
+        <v>213</v>
+      </c>
+      <c r="H3" s="4" t="inlineStr">
+        <is>
+          <t>4 В</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>Сапаров Айбек Галымжанович</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>010101854353</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>Сапаров Галымжан Талгатович</t>
+        </is>
+      </c>
+      <c r="E4" s="4" t="inlineStr">
+        <is>
+          <t>+7 (771) 168-86-87</t>
+        </is>
+      </c>
+      <c r="F4" s="4" t="inlineStr">
+        <is>
+          <t>Ораза Татеулы 13А</t>
+        </is>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>80000</v>
+      </c>
+      <c r="H4" s="4" t="inlineStr">
+        <is>
+          <t>6 А</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="F7" s="5" t="inlineStr">
+        <is>
+          <t>Все классы - 3 учеников</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
SUPER HUGE COMMIT FROM THE SERVER
</commit_message>
<xml_diff>
--- a/staticfiles/user_manager/students.xlsx
+++ b/staticfiles/user_manager/students.xlsx
@@ -2,11 +2,12 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Все классы" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="9C класс" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,19 +26,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <family val="2"/>
       <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b val="1"/>
       <color rgb="00FFFFFF"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -63,19 +56,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
     <border>
       <left style="thin">
@@ -107,12 +91,12 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -475,9 +459,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -529,11 +513,6 @@
           <t>Оплата</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
-        <is>
-          <t>Класс</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
@@ -541,36 +520,31 @@
       </c>
       <c r="B2" s="4" t="inlineStr">
         <is>
-          <t>erwyg dfgs dfgs</t>
+          <t>Айдашева Айзере Темирбековна</t>
         </is>
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>856477567657</t>
+          <t>110802603492</t>
         </is>
       </c>
       <c r="D2" s="4" t="inlineStr">
         <is>
-          <t>dfsa ddafs asdf</t>
+          <t>Айдашева Гульзат Аслановна</t>
         </is>
       </c>
       <c r="E2" s="4" t="inlineStr">
         <is>
-          <t>+7 (132) 412-34-31</t>
+          <t>+7 (701) 556-54-58</t>
         </is>
       </c>
       <c r="F2" s="4" t="inlineStr">
         <is>
-          <t>sadf</t>
+          <t>Алтын орда 19 кв 57</t>
         </is>
       </c>
       <c r="G2" s="4" t="n">
-        <v>3124</v>
-      </c>
-      <c r="H2" s="4" t="inlineStr">
-        <is>
-          <t>3 Б</t>
-        </is>
+        <v>35000</v>
       </c>
     </row>
     <row r="3">
@@ -579,34 +553,31 @@
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t>Baismakova Danochka Samatovna</t>
+          <t>Базарбай Нұртас Құрманбекұлы</t>
         </is>
       </c>
       <c r="C3" s="4" t="inlineStr">
         <is>
-          <t>000612693204</t>
+          <t>100509552658</t>
         </is>
       </c>
       <c r="D3" s="4" t="inlineStr">
         <is>
-          <t>ауцауц уцауц уацауц</t>
+          <t xml:space="preserve">Ешмагамбетова Айнур </t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
         <is>
-          <t>+7 (777) 025-52-00</t>
+          <t>+7 (771) 828-33-44</t>
         </is>
       </c>
       <c r="F3" s="4" t="inlineStr">
         <is>
-          <t>аыппа</t>
-        </is>
-      </c>
-      <c r="G3" s="4" t="n"/>
-      <c r="H3" s="4" t="inlineStr">
-        <is>
-          <t>4 Ә</t>
-        </is>
+          <t>Мустафа Шокай 48В к1 кв 18</t>
+        </is>
+      </c>
+      <c r="G3" s="4" t="n">
+        <v>147600</v>
       </c>
     </row>
     <row r="4">
@@ -615,36 +586,31 @@
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dolmagambetov Karen </t>
+          <t>Базарқұл Гүлназ Аманқұлқызы</t>
         </is>
       </c>
       <c r="C4" s="4" t="inlineStr">
         <is>
-          <t>010608550491</t>
+          <t>111043602043</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
         <is>
-          <t>Долмагамбетов Талгат Аманжолович</t>
+          <t>Махамбетова Жаннұр Казиевна</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
         <is>
-          <t>+7 (771) 168-86-87</t>
+          <t>+7 (708) 176-94-96</t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
         <is>
-          <t>214234</t>
+          <t>Құрмашев 28</t>
         </is>
       </c>
       <c r="G4" s="4" t="n">
-        <v>213</v>
-      </c>
-      <c r="H4" s="4" t="inlineStr">
-        <is>
-          <t>4 В</t>
-        </is>
+        <v>25000</v>
       </c>
     </row>
     <row r="5">
@@ -653,46 +619,338 @@
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t>Сапаров Айбек Галымжанович</t>
+          <t>Батырбаева Айлин Еркиновна</t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
         <is>
-          <t>010101854353</t>
+          <t>120719603413</t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
         <is>
-          <t>Сапаров Галымжан Талгатович</t>
+          <t>Батырбаева Гулсамал Есеновна</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
         <is>
-          <t>+7 (702) 827-25-62</t>
+          <t>+7 (707) 883-37-33</t>
         </is>
       </c>
       <c r="F5" s="4" t="inlineStr">
         <is>
-          <t>Ораза Татеулы 13А</t>
+          <t>Ветеран 2 д31</t>
         </is>
       </c>
       <c r="G5" s="4" t="n">
-        <v>80000</v>
-      </c>
-      <c r="H5" s="4" t="inlineStr">
-        <is>
-          <t>6 А</t>
-        </is>
+        <v>81000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>Жумакаева Молдир Бахадыровна</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>101130602600</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ермагамбетова Диляра </t>
+        </is>
+      </c>
+      <c r="E6" s="4" t="inlineStr">
+        <is>
+          <t>+7 (705) 473-60-75</t>
+        </is>
+      </c>
+      <c r="F6" s="4" t="inlineStr">
+        <is>
+          <t>уч №143 Шабыт 124</t>
+        </is>
+      </c>
+      <c r="G6" s="4" t="n">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>Изтилеу Аяулым Асхатқызы</t>
+        </is>
+      </c>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t>110813603790</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="inlineStr">
+        <is>
+          <t>сейлханова Рысгул Мирхановна</t>
+        </is>
+      </c>
+      <c r="E7" s="4" t="inlineStr">
+        <is>
+          <t>+7 (701) 615-70-79</t>
+        </is>
+      </c>
+      <c r="F7" s="4" t="inlineStr">
+        <is>
+          <t>м.шоқай71</t>
+        </is>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>50000</v>
       </c>
     </row>
     <row r="8">
-      <c r="F8" s="5" t="inlineStr">
-        <is>
-          <t>Все классы - 4 учеников</t>
+      <c r="A8" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>Муслимова Ляйсан Дамировна</t>
+        </is>
+      </c>
+      <c r="C8" s="4" t="inlineStr">
+        <is>
+          <t>110518603617</t>
+        </is>
+      </c>
+      <c r="D8" s="4" t="inlineStr">
+        <is>
+          <t>Муслимова Динара Тлеповна</t>
+        </is>
+      </c>
+      <c r="E8" s="4" t="inlineStr">
+        <is>
+          <t>+7 (777) 817-32-96</t>
+        </is>
+      </c>
+      <c r="F8" s="4" t="inlineStr">
+        <is>
+          <t>Батыс 2 дом 7 корпус 4</t>
+        </is>
+      </c>
+      <c r="G8" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>Назарбаева Лана Данияровна</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="inlineStr">
+        <is>
+          <t>100914653238</t>
+        </is>
+      </c>
+      <c r="D9" s="4" t="inlineStr">
+        <is>
+          <t>Назарбаева Асель Маратовна</t>
+        </is>
+      </c>
+      <c r="E9" s="4" t="inlineStr">
+        <is>
+          <t>+7 (701) 920-30-48</t>
+        </is>
+      </c>
+      <c r="F9" s="4" t="inlineStr">
+        <is>
+          <t>Саздинское лесничество 197а, кв3</t>
+        </is>
+      </c>
+      <c r="G9" s="4" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t>Орынбасар Аянат Дулаткызы</t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t>110125602593</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t>Құдайбергенова Әсел Әлибекқызы</t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t>+7 (702) 106-56-85</t>
+        </is>
+      </c>
+      <c r="F10" s="4" t="inlineStr">
+        <is>
+          <t>Мангилик ел 5, к4, кв10</t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="n">
+        <v>102000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="inlineStr">
+        <is>
+          <t>Өтеп Әмина Нұрасханқызы</t>
+        </is>
+      </c>
+      <c r="C11" s="4" t="inlineStr">
+        <is>
+          <t>110218604684</t>
+        </is>
+      </c>
+      <c r="D11" s="4" t="inlineStr">
+        <is>
+          <t>Танирбергенова Айгүл Ельбаевна</t>
+        </is>
+      </c>
+      <c r="E11" s="4" t="inlineStr">
+        <is>
+          <t>+7 (705) 474-77-84</t>
+        </is>
+      </c>
+      <c r="F11" s="4" t="inlineStr">
+        <is>
+          <t>Жаңақоныс, Инабат 22</t>
+        </is>
+      </c>
+      <c r="G11" s="4" t="n">
+        <v>43700</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="inlineStr">
+        <is>
+          <t>Пирвердиева Тамила Заургызы</t>
+        </is>
+      </c>
+      <c r="C12" s="4" t="inlineStr">
+        <is>
+          <t>110125603660</t>
+        </is>
+      </c>
+      <c r="D12" s="4" t="inlineStr">
+        <is>
+          <t>Пирвердиева Динара Муханбетовна</t>
+        </is>
+      </c>
+      <c r="E12" s="4" t="inlineStr">
+        <is>
+          <t>+7 (702) 201-05-50</t>
+        </is>
+      </c>
+      <c r="F12" s="4" t="inlineStr">
+        <is>
+          <t>Акжар - 2, Райымбек батыра 8</t>
+        </is>
+      </c>
+      <c r="G12" s="4" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="inlineStr">
+        <is>
+          <t>Шахаров Әлинур Асхатұлы</t>
+        </is>
+      </c>
+      <c r="C13" s="4" t="inlineStr">
+        <is>
+          <t>110221500831</t>
+        </is>
+      </c>
+      <c r="D13" s="4" t="inlineStr">
+        <is>
+          <t>Шахарова Алия Булаткалиевна</t>
+        </is>
+      </c>
+      <c r="E13" s="4" t="inlineStr">
+        <is>
+          <t>+7 (701) 554-04-99</t>
+        </is>
+      </c>
+      <c r="F13" s="4" t="inlineStr">
+        <is>
+          <t>Сәңкібай батыр көшесі, 28Вк3, 36 пәтер</t>
+        </is>
+      </c>
+      <c r="G13" s="4" t="n">
+        <v>38000</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="inlineStr">
+        <is>
+          <t>Шаяхмет Дәулет Мирланұлы</t>
+        </is>
+      </c>
+      <c r="C14" s="4" t="inlineStr">
+        <is>
+          <t>101112502745</t>
+        </is>
+      </c>
+      <c r="D14" s="4" t="inlineStr">
+        <is>
+          <t>Едилова Динара Ерсаиновна</t>
+        </is>
+      </c>
+      <c r="E14" s="4" t="inlineStr">
+        <is>
+          <t>+7 (701) 222-17-86</t>
+        </is>
+      </c>
+      <c r="F14" s="4" t="inlineStr">
+        <is>
+          <t>Ғ.жубанова 83</t>
+        </is>
+      </c>
+      <c r="G14" s="4" t="n">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="F17" s="5" t="inlineStr">
+        <is>
+          <t>9C класс - 13 учеников</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>